<commit_message>
chỉnh excel cho đẹp
</commit_message>
<xml_diff>
--- a/danso.xlsx
+++ b/danso.xlsx
@@ -432,6 +432,20 @@
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <cols>
+    <col width="5" customWidth="1" min="1" max="1"/>
+    <col width="15" customWidth="1" min="2" max="2"/>
+    <col width="20" customWidth="1" min="3" max="3"/>
+    <col width="13" customWidth="1" min="4" max="4"/>
+    <col width="12" customWidth="1" min="5" max="5"/>
+    <col width="15" customWidth="1" min="6" max="6"/>
+    <col width="10" customWidth="1" min="7" max="7"/>
+    <col width="18" customWidth="1" min="8" max="8"/>
+    <col width="22" customWidth="1" min="9" max="9"/>
+    <col width="22" customWidth="1" min="10" max="10"/>
+    <col width="10" customWidth="1" min="11" max="11"/>
+    <col width="14" customWidth="1" min="12" max="12"/>
+  </cols>
   <sheetData>
     <row r="1">
       <c r="B1" s="1" t="inlineStr">

</xml_diff>